<commit_message>
[TAN-1834] Fix bug where idea dataa leaked into empty rows
</commit_message>
<xml_diff>
--- a/back/engines/commercial/bulk_import_ideas/spec/fixtures/import.xlsx
+++ b/back/engines/commercial/bulk_import_ideas/spec/fixtures/import.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Full name</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>A custom field</t>
+    <t>Text field</t>
   </si>
   <si>
     <t>Image URL</t>
@@ -70,6 +70,9 @@
     <t>Oxford</t>
   </si>
   <si>
+    <t>Some custom text here</t>
+  </si>
+  <si>
     <t>https://cl2-seed-and-template-assets.s3.eu-central-1.amazonaws.com/images/people_in_meeting_graphic.png</t>
   </si>
   <si>
@@ -85,7 +88,7 @@
     <t>And another description here</t>
   </si>
   <si>
-    <t>Some custom text here</t>
+    <t>Cambridge</t>
   </si>
 </sst>
 </file>
@@ -1310,9 +1313,11 @@
       <c r="H2" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" t="s" s="3">
+        <v>19</v>
+      </c>
       <c r="J2" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="5">
         <v>50.5035</v>
@@ -1323,10 +1328,10 @@
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="3">
         <v>14</v>
@@ -1335,20 +1340,18 @@
         <v>15</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s" s="3">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I3" s="3"/>
       <c r="J3" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K3" s="5">
         <v>50.5035</v>

</xml_diff>